<commit_message>
using LoadFromCollection to load stats into spreadsheet
</commit_message>
<xml_diff>
--- a/3/CakeExtracter.ConsoleApplication/SearchPPCtemplate.xlsx
+++ b/3/CakeExtracter.ConsoleApplication/SearchPPCtemplate.xlsx
@@ -507,8 +507,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="60063104"/>
-        <c:axId val="64435712"/>
+        <c:axId val="64460288"/>
+        <c:axId val="73516544"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -652,11 +652,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="67560960"/>
-        <c:axId val="64437248"/>
+        <c:axId val="73844224"/>
+        <c:axId val="73518080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="60063104"/>
+        <c:axId val="64460288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -666,7 +666,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64435712"/>
+        <c:crossAx val="73516544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -674,7 +674,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64435712"/>
+        <c:axId val="73516544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,12 +685,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60063104"/>
+        <c:crossAx val="64460288"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64437248"/>
+        <c:axId val="73518080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -700,12 +700,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67560960"/>
+        <c:crossAx val="73844224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="67560960"/>
+        <c:axId val="73844224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -715,7 +715,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="64437248"/>
+        <c:crossAx val="73518080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1357,7 +1357,7 @@
   <dimension ref="B8:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,7 +1369,7 @@
     <col min="7" max="7" width="15.85546875" style="1" customWidth="1"/>
     <col min="8" max="9" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" style="1" customWidth="1"/>
     <col min="12" max="13" width="9.140625" style="1"/>
     <col min="14" max="14" width="9.140625" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="1"/>

</xml_diff>

<commit_message>
generate a chart in the spreadsheet
</commit_message>
<xml_diff>
--- a/3/CakeExtracter.ConsoleApplication/SearchPPCtemplate.xlsx
+++ b/3/CakeExtracter.ConsoleApplication/SearchPPCtemplate.xlsx
@@ -11,9 +11,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -330,425 +327,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="121"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="21"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Weekly Performance 2014</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="4.3245531733493672E-2"/>
-          <c:y val="0.83504127579042564"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="1"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="4.0221803195040776E-2"/>
-          <c:y val="0.11712735024132839"/>
-          <c:w val="0.89361278806110656"/>
-          <c:h val="0.53505233758660298"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'[1]Week to Week-Hide'!$A$28</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Revenue</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'[1]Executive Summary'!$B$79:$B$91</c:f>
-              <c:strCache>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>6/11- 6/17</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6/18 - 6/24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6/25 - 7/1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7/2 - 7/8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7/9 - 7/15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7/16 - 7/22</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7/23 - 7/29</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7/30 - 8/5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8/6 - 8/12</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8/13 - 8/19</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8/20 - 8/26</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8/27 - 9/2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9/3 - 9/9</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'[1]Executive Summary'!$I$79:$I$91</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>105842.53999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>101901.04</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>94423.34</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>104824.69</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>114056.32000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>108813.17</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>85971.31</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>75932.75</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>63849.789999999994</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>58742.229999999996</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>104072.76000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>114094.13999999998</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>99818.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="64460288"/>
-        <c:axId val="73516544"/>
-      </c:barChart>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'[1]Executive Summary'!$C$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Clicks</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'[1]Executive Summary'!$B$79:$B$91</c:f>
-              <c:strCache>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>6/11- 6/17</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6/18 - 6/24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6/25 - 7/1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7/2 - 7/8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7/9 - 7/15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7/16 - 7/22</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7/23 - 7/29</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7/30 - 8/5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8/6 - 8/12</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8/13 - 8/19</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8/20 - 8/26</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8/27 - 9/2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9/3 - 9/9</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'[1]Executive Summary'!$C$79:$C$91</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>58933</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>44970</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>51786</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>47323</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50793</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>51611</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>53885</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>57082</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>47581</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45212</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>51134</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>54464</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>52856</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="73844224"/>
-        <c:axId val="73518080"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="64460288"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="[$-409]d\-mmm;@" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73516544"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="0"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="73516544"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="r"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64460288"/>
-        <c:crosses val="max"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="73518080"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73844224"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:catAx>
-        <c:axId val="73844224"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="none"/>
-        <c:crossAx val="73518080"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="0"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.85740406203998865"/>
-          <c:y val="0.85846237033031747"/>
-          <c:w val="0.13471895767402475"/>
-          <c:h val="9.4502857269835205E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001565" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000001565" header="0.30000000000000032" footer="0.30000000000000032"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -793,278 +371,7 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>187404</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="http://answ-merchlogos.s3.amazonaws.com/20111219/29593_folica_logo.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9448800" y="2047875"/>
-          <a:ext cx="1457325" cy="235029"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>552451</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>79653</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Executive Summary"/>
-      <sheetName val="Week to Week-Hide"/>
-      <sheetName val="Month to Month-Hide"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Criteo"/>
-      <sheetName val="Criteo Breakdown"/>
-      <sheetName val="Recent Brand Analysis"/>
-      <sheetName val="Criteo Monthly"/>
-      <sheetName val="Google WoW"/>
-      <sheetName val="Ad Copy Test"/>
-      <sheetName val="Experiments Summary"/>
-      <sheetName val="GA - Data"/>
-      <sheetName val="Action Item"/>
-      <sheetName val="Paid Search Steps-HIDE"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="8">
-          <cell r="C8" t="str">
-            <v>Clicks</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="B79" t="str">
-            <v>6/11- 6/17</v>
-          </cell>
-          <cell r="C79">
-            <v>58933</v>
-          </cell>
-          <cell r="I79">
-            <v>105842.53999999998</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="B80" t="str">
-            <v>6/18 - 6/24</v>
-          </cell>
-          <cell r="C80">
-            <v>44970</v>
-          </cell>
-          <cell r="I80">
-            <v>101901.04</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="B81" t="str">
-            <v>6/25 - 7/1</v>
-          </cell>
-          <cell r="C81">
-            <v>51786</v>
-          </cell>
-          <cell r="I81">
-            <v>94423.34</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="B82" t="str">
-            <v>7/2 - 7/8</v>
-          </cell>
-          <cell r="C82">
-            <v>47323</v>
-          </cell>
-          <cell r="I82">
-            <v>104824.69</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="B83" t="str">
-            <v>7/9 - 7/15</v>
-          </cell>
-          <cell r="C83">
-            <v>50793</v>
-          </cell>
-          <cell r="I83">
-            <v>114056.32000000001</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="B84" t="str">
-            <v>7/16 - 7/22</v>
-          </cell>
-          <cell r="C84">
-            <v>51611</v>
-          </cell>
-          <cell r="I84">
-            <v>108813.17</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="B85" t="str">
-            <v>7/23 - 7/29</v>
-          </cell>
-          <cell r="C85">
-            <v>53885</v>
-          </cell>
-          <cell r="I85">
-            <v>85971.31</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="B86" t="str">
-            <v>7/30 - 8/5</v>
-          </cell>
-          <cell r="C86">
-            <v>57082</v>
-          </cell>
-          <cell r="I86">
-            <v>75932.75</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="B87" t="str">
-            <v>8/6 - 8/12</v>
-          </cell>
-          <cell r="C87">
-            <v>47581</v>
-          </cell>
-          <cell r="I87">
-            <v>63849.789999999994</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="B88" t="str">
-            <v>8/13 - 8/19</v>
-          </cell>
-          <cell r="C88">
-            <v>45212</v>
-          </cell>
-          <cell r="I88">
-            <v>58742.229999999996</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="B89" t="str">
-            <v>8/20 - 8/26</v>
-          </cell>
-          <cell r="C89">
-            <v>51134</v>
-          </cell>
-          <cell r="I89">
-            <v>104072.76000000001</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="B90" t="str">
-            <v>8/27 - 9/2</v>
-          </cell>
-          <cell r="C90">
-            <v>54464</v>
-          </cell>
-          <cell r="I90">
-            <v>114094.13999999998</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="B91" t="str">
-            <v>9/3 - 9/9</v>
-          </cell>
-          <cell r="C91">
-            <v>52856</v>
-          </cell>
-          <cell r="I91">
-            <v>99818.9</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="24">
-          <cell r="CU24">
-            <v>58933</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>Revenue</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1357,7 +664,7 @@
   <dimension ref="B8:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>